<commit_message>
feature: Allow shorter factor lists but enabling exclusion of composites (seems to break Streamlit app)
</commit_message>
<xml_diff>
--- a/risk_lib/factor_master.xlsx
+++ b/risk_lib/factor_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrai\Source\risk\risk_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B492B03-0CC0-4B15-B78A-A924D753610B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A550DB0-E25E-4E50-BFD9-FF4AD6658C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="5" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="4" activeTab="11" xr2:uid="{C31FDC5B-A809-4BFD-99CB-DA02246721F7}"/>
   </bookViews>
   <sheets>
     <sheet name="legacy" sheetId="5" r:id="rId1"/>
@@ -1616,7 +1616,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1676,7 +1676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1695,15 +1695,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -5852,7 +5844,7 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8079,7 +8071,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B51E7A-08A5-4042-86E1-7986ED98437B}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -8088,40 +8082,32 @@
         <f>read!A1</f>
         <v>factor_name</v>
       </c>
-      <c r="B1" t="str">
-        <f>read!B1</f>
+      <c r="B1" t="str" cm="1">
+        <f t="array" ref="B1:J1">_xlfn.DROP(_xlfn.TRIMRANGE(read!1:1),,1)</f>
         <v>asset_class</v>
       </c>
       <c r="C1" t="str">
-        <f>read!C1</f>
         <v>region</v>
       </c>
       <c r="D1" t="str">
-        <f>read!D1</f>
         <v>hyper_factor</v>
       </c>
       <c r="E1" t="str">
-        <f>read!E1</f>
         <v>composite</v>
       </c>
       <c r="F1" t="str">
-        <f>read!F1</f>
         <v>description</v>
       </c>
       <c r="G1" t="str">
-        <f>read!G1</f>
         <v>source</v>
       </c>
       <c r="H1" t="str">
-        <f>read!H1</f>
         <v>ticker</v>
       </c>
       <c r="I1" t="str">
-        <f>read!I1</f>
         <v>diffusion_type</v>
       </c>
       <c r="J1" t="str">
-        <f>read!J1</f>
         <v>multiplier</v>
       </c>
     </row>
@@ -8131,7 +8117,7 @@
         <v>SPY</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:J6">_xlfn.CHOOSEROWS(_xlfn.ANCHORARRAY(read!B2),_xlfn.SEQUENCE(5))</f>
+        <f t="array" ref="B2:J6">INDEX(data[],_xlfn.XMATCH(_xlfn.ANCHORARRAY(A2),data[factor_name]),_xlfn.XMATCH(_xlfn.ANCHORARRAY(B1),data[#Headers]))</f>
         <v>Equities</v>
       </c>
       <c r="C2" t="str">
@@ -14587,9 +14573,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -14847,8 +14831,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14856,8 +14840,6 @@
     <col min="1" max="1" width="15.44140625" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="9"/>
-    <col min="8" max="8" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -15206,14 +15188,14 @@
         <v>441</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>505</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" t="s">
         <v>182</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="8">
         <v>1</v>
       </c>
       <c r="E15">
@@ -15222,150 +15204,148 @@
       <c r="G15" t="s">
         <v>505</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15">
         <v>22</v>
       </c>
-      <c r="K15" s="9" t="b">
+      <c r="K15" t="b">
         <f ca="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>505</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" t="s">
         <v>178</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="8">
         <v>-1</v>
       </c>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="H16" s="9">
+      <c r="H16">
         <v>16</v>
       </c>
-      <c r="K16" s="9" t="b">
+      <c r="K16" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>502</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="12" cm="1">
+      <c r="C17" s="8" cm="1">
         <f t="array" ref="C17">E17/D17*$F$17/SUM(ABS(($E$17:$E$21)))</f>
         <v>0.20547945205479451</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17">
         <v>14.6</v>
       </c>
-      <c r="E17" s="9">
-        <v>1</v>
-      </c>
-      <c r="F17" s="13">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="9">
         <v>15</v>
       </c>
-      <c r="J17" s="9" cm="1">
+      <c r="J17" cm="1">
         <f t="array" ref="J17:J20">C17:C20*D17:D20</f>
         <v>2.9999999999999996</v>
       </c>
-      <c r="K17" s="9" t="b">
+      <c r="K17" t="b">
         <f ca="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>502</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="8">
         <f>E18/D18*$F$17/COUNT($E$17:$E$21)</f>
         <v>0.29702970297029702</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18">
         <v>10.1</v>
       </c>
-      <c r="E18" s="9">
-        <v>1</v>
-      </c>
-      <c r="J18" s="9">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="J18">
         <v>2.9999999999999996</v>
       </c>
-      <c r="K18" s="9" t="b">
+      <c r="K18" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>502</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" t="s">
         <v>499</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="8">
         <f>E19/D19*$F$17/COUNT($E$17:$E$21)</f>
         <v>0.36585365853658536</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E19" s="9">
-        <v>1</v>
-      </c>
-      <c r="J19" s="9">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="J19">
         <v>2.9999999999999996</v>
       </c>
-      <c r="K19" s="9" t="b">
+      <c r="K19" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
-      <c r="M19" s="9" t="s">
+      <c r="M19" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>502</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" t="s">
         <v>497</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="8">
         <f>E20/D20*$F$17/COUNT($E$17:$E$21)</f>
         <v>-3.7499999999999999E-2</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20">
         <v>80</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20">
         <v>-1</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20">
         <v>-3</v>
       </c>
-      <c r="K20" s="9" t="b">
+      <c r="K20" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+      <c r="A21" t="s">
         <v>502</v>
       </c>
-      <c r="B21" s="9" t="str">
+      <c r="B21" t="str">
         <f t="shared" ref="B21:B22" si="0">B15</f>
         <v>XLP</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="8">
         <f>E21/D21*$F$17/COUNT($E$17:$E$21)</f>
         <v>0.15</v>
       </c>
@@ -15381,40 +15361,24 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="A22" t="s">
         <v>502</v>
       </c>
-      <c r="B22" s="9" t="str">
+      <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v>XLY</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="8">
         <f>-C21</f>
         <v>-0.15</v>
       </c>
-      <c r="D22" s="9"/>
       <c r="K22" t="b">
         <f ca="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C26" s="9"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C27" s="9"/>
+      <c r="C23" s="8"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -15445,7 +15409,7 @@
       <c r="B29" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="8">
         <f>E29/D29</f>
         <v>0.29702970297029702</v>
       </c>
@@ -15466,7 +15430,7 @@
       <c r="B30" t="s">
         <v>499</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="8">
         <f>E30/D30</f>
         <v>0.36585365853658541</v>
       </c>
@@ -15487,10 +15451,10 @@
       <c r="A31" t="s">
         <v>506</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" t="s">
         <v>497</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="8">
         <f>E31/D31</f>
         <v>-0.1125</v>
       </c>
@@ -15506,14 +15470,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:C14 A15:A16 C15:C16 B15 A28:C31">
+  <conditionalFormatting sqref="A2:C14 B15 A15:A16 C15:C16 A28:C31">
     <cfRule type="expression" dxfId="8" priority="5">
       <formula>$K2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:C22 B21">
-    <cfRule type="expression" dxfId="7" priority="21">
-      <formula>$K19</formula>
+  <conditionalFormatting sqref="A17:C17 B18:C20 A18:A22 C21">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>$K17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:C23">
@@ -15521,9 +15485,9 @@
       <formula>$K16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:C17 C21 B18:C20 A18:A22">
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>$K17</formula>
+  <conditionalFormatting sqref="B21 B22:C22">
+    <cfRule type="expression" dxfId="5" priority="21">
+      <formula>$K19</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20048,129 +20012,128 @@
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A86" s="10" t="s">
+      <c r="A86" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="B86" s="10" t="s">
+      <c r="B86" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C86" s="10" t="s">
+      <c r="C86" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="10"/>
-      <c r="G86" s="10"/>
-      <c r="H86" s="10">
-        <v>1</v>
-      </c>
-      <c r="I86" s="10">
-        <v>1</v>
-      </c>
-      <c r="J86" s="10">
-        <v>1</v>
-      </c>
-      <c r="K86" s="10">
-        <v>0</v>
-      </c>
-      <c r="L86" s="11">
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4">
+        <v>1</v>
+      </c>
+      <c r="I86" s="4">
+        <v>1</v>
+      </c>
+      <c r="J86" s="4">
+        <v>1</v>
+      </c>
+      <c r="K86" s="4">
+        <v>0</v>
+      </c>
+      <c r="L86" s="4">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>0</v>
       </c>
-      <c r="M86" s="10" t="s">
+      <c r="M86" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="N86" s="10" t="s">
+      <c r="N86" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="O86" s="11" cm="1">
+      <c r="O86" s="4" cm="1">
         <f t="array" ref="O86">_xlfn.SWITCH(data[[#This Row],[diffusion_type]],"lognormal",0.0001,"normal",-0.01)*IF(data[[#This Row],[asset_class]]="Vol",-1,1)</f>
         <v>1E-4</v>
       </c>
-      <c r="P86" s="11" t="str">
+      <c r="P86" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
         <v>XLPXLY</v>
       </c>
-      <c r="Q86" s="11"/>
-      <c r="R86" s="9"/>
-      <c r="S86" s="9" t="b">
+      <c r="Q86" s="4"/>
+      <c r="S86" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A87" s="10" t="s">
+      <c r="A87" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="B87" s="10" t="s">
+      <c r="B87" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C87" s="10" t="s">
+      <c r="C87" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="D87" s="10"/>
-      <c r="E87" s="10"/>
-      <c r="F87" s="10"/>
-      <c r="G87" s="10"/>
-      <c r="H87" s="10">
-        <v>1</v>
-      </c>
-      <c r="I87" s="10">
-        <v>1</v>
-      </c>
-      <c r="J87" s="10">
-        <v>1</v>
-      </c>
-      <c r="K87" s="10">
-        <v>0</v>
-      </c>
-      <c r="L87" s="11">
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4">
+        <v>1</v>
+      </c>
+      <c r="I87" s="4">
+        <v>1</v>
+      </c>
+      <c r="J87" s="4">
+        <v>1</v>
+      </c>
+      <c r="K87" s="4">
+        <v>0</v>
+      </c>
+      <c r="L87" s="4">
         <f>IF(data[[#This Row],[description_override]]="",data[[#This Row],[Description_GPT]],data[[#This Row],[description_override]])</f>
         <v>0</v>
       </c>
-      <c r="M87" s="10" t="s">
+      <c r="M87" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="N87" s="10" t="s">
+      <c r="N87" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="O87" s="11" cm="1">
+      <c r="O87" s="4" cm="1">
         <f t="array" ref="O87">_xlfn.SWITCH(data[[#This Row],[diffusion_type]],"lognormal",0.0001,"normal",-0.01)*IF(data[[#This Row],[asset_class]]="Vol",-1,1)</f>
         <v>1E-4</v>
       </c>
-      <c r="P87" s="11" t="str">
+      <c r="P87" s="4" t="str">
         <f>data[[#This Row],[factor_name]]</f>
         <v>TRADEWAR</v>
       </c>
-      <c r="Q87" s="11"/>
+      <c r="Q87" s="4"/>
       <c r="S87" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="A86:B86 H86:K86 M86:N86">
+    <cfRule type="expression" dxfId="4" priority="24">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A2:Q65 A68:Q72">
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>$S2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A67:Q67 A76:Q85 A73:Q74 A87:B87 H87:K87 M87:N87">
-    <cfRule type="expression" dxfId="3" priority="12">
-      <formula>$S66</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66:Q66">
+  <conditionalFormatting sqref="A66:Q67">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$S65</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A75:Q75">
-    <cfRule type="expression" dxfId="1" priority="14">
-      <formula>$S73</formula>
+  <conditionalFormatting sqref="A73:Q74 A76:Q85 A87:B87 H87:K87 M87:N87">
+    <cfRule type="expression" dxfId="1" priority="12">
+      <formula>$S72</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A86:B86 H86:K86 M86:N86">
-    <cfRule type="expression" dxfId="0" priority="24">
-      <formula>#REF!</formula>
+  <conditionalFormatting sqref="A75:Q75">
+    <cfRule type="expression" dxfId="0" priority="14">
+      <formula>$S73</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>